<commit_message>
added tables with data
</commit_message>
<xml_diff>
--- a/cv_09/data/dvora135_EMB-cv_09_data.xlsx
+++ b/cv_09/data/dvora135_EMB-cv_09_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvorakj/Disk Google/Sdílené složky/Škola_shared/3_semestr/EMB/Cv/Protokoly/cv_09/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5265DE24-A1BA-3842-99D9-62998E1DB703}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC18201-B30F-3641-8A37-FC9A897E10D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="2400" windowWidth="27640" windowHeight="16860" xr2:uid="{33BC4E61-6734-2943-AA4E-0C25C1BD067A}"/>
+    <workbookView xWindow="5580" yWindow="3600" windowWidth="27640" windowHeight="16860" xr2:uid="{33BC4E61-6734-2943-AA4E-0C25C1BD067A}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,62 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+  <si>
+    <t>60 Hz [Hz]</t>
+  </si>
+  <si>
+    <t>10 kHz [kHz]</t>
+  </si>
+  <si>
+    <t>100 kHz [kHz]</t>
+  </si>
+  <si>
+    <t>0,1 s</t>
+  </si>
+  <si>
+    <t>1 s</t>
+  </si>
+  <si>
+    <t>10 s</t>
+  </si>
+  <si>
+    <t>60 Hz [s]</t>
+  </si>
+  <si>
+    <t>10 kHz [s]</t>
+  </si>
+  <si>
+    <t>100 kHz [s]</t>
+  </si>
+  <si>
+    <t>1 T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 T </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>100 T</t>
+  </si>
+  <si>
+    <t>1000 T</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>f [kHz]</t>
+  </si>
+  <si>
+    <t>T [us]</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,14 +436,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E48717-D610-F845-9E61-63835B65E6EC}">
-  <dimension ref="A1"/>
+  <dimension ref="F5:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>70</v>
+      </c>
+      <c r="H6">
+        <v>10.63</v>
+      </c>
+      <c r="I6">
+        <v>110.83</v>
+      </c>
+    </row>
+    <row r="7" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>68</v>
+      </c>
+      <c r="H7">
+        <v>10.622</v>
+      </c>
+      <c r="I7">
+        <v>110.828</v>
+      </c>
+    </row>
+    <row r="8" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="H8">
+        <v>10.623100000000001</v>
+      </c>
+      <c r="I8">
+        <v>110.8373</v>
+      </c>
+    </row>
+    <row r="10" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>15100.7</v>
+      </c>
+      <c r="H11">
+        <v>93.6</v>
+      </c>
+      <c r="I11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>15101.87</v>
+      </c>
+      <c r="H12">
+        <v>93.64</v>
+      </c>
+      <c r="I12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>93.648799999999994</v>
+      </c>
+      <c r="I13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14">
+        <v>93.636330000000001</v>
+      </c>
+      <c r="I14">
+        <v>9.0555299999999992</v>
+      </c>
+    </row>
+    <row r="15" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>32.767699999999998</v>
+      </c>
+      <c r="H19">
+        <v>2000038.9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>